<commit_message>
vault backup: 2024-08-28 21:24:41
</commit_message>
<xml_diff>
--- a/2024-2/Evaluación de proyectos/Excels/Estudio_C1.xlsx
+++ b/2024-2/Evaluación de proyectos/Excels/Estudio_C1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IVAN\Desktop\Codes\Apuntes_2024\2024-2\Evaluación de proyectos\Excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C82AD091-7735-4C49-BF33-B06AE34A2768}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36655C6D-B7B1-4759-B779-5E20135431FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2E2B48C4-17E3-4387-8B2C-BD530D7BDFF8}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="69">
   <si>
     <t>AYUDANTÍA</t>
   </si>
@@ -184,6 +184,66 @@
   </si>
   <si>
     <t>JUBILACIÓN</t>
+  </si>
+  <si>
+    <t>Expectativa de vida</t>
+  </si>
+  <si>
+    <t>Sueldo mensual</t>
+  </si>
+  <si>
+    <t>13% AFP</t>
+  </si>
+  <si>
+    <t>7% Isapre</t>
+  </si>
+  <si>
+    <t>Sueldo descontado</t>
+  </si>
+  <si>
+    <t>Impuesto 10%</t>
+  </si>
+  <si>
+    <t>Sueldo liquido</t>
+  </si>
+  <si>
+    <t>VIDA LABORAL (AÑOS)</t>
+  </si>
+  <si>
+    <t>VIDA LABORAL (MESES)</t>
+  </si>
+  <si>
+    <t>AÑOS JUBILACION</t>
+  </si>
+  <si>
+    <t>MESES JUBILACION</t>
+  </si>
+  <si>
+    <t>FONDO ACUMULADO JUBILACION</t>
+  </si>
+  <si>
+    <t>RENTABILIDAD AFP AL MES</t>
+  </si>
+  <si>
+    <t>JUBILACION MENSUAL</t>
+  </si>
+  <si>
+    <t>MONTO ADICIONAL DESEADO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HOMBRE </t>
+  </si>
+  <si>
+    <t>JUBILACIÓN DESEADA</t>
+  </si>
+  <si>
+    <t>FONDO ACUMULADO DESEADO</t>
+  </si>
+  <si>
+    <t>MONTO AFP POR MES</t>
+  </si>
+  <si>
+    <t>INCREMENTO AL FONDO PREVISIONAL</t>
   </si>
 </sst>
 </file>
@@ -272,7 +332,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="22">
+  <borders count="28">
     <border>
       <left/>
       <right/>
@@ -559,128 +619,106 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="105">
+  <cellXfs count="115">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="6" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="6" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="6" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
@@ -689,18 +727,6 @@
     <xf numFmtId="8" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="12" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -713,68 +739,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="42" fontId="0" fillId="2" borderId="21" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="6" fontId="0" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="8" fontId="0" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="6" fontId="0" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="9" fontId="0" fillId="4" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="6" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="6" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="8" fontId="0" fillId="5" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
@@ -783,16 +760,195 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="8" fontId="0" fillId="2" borderId="21" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="8" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="8" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="8" fontId="0" fillId="2" borderId="21" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Moneda [0]" xfId="1" builtinId="7"/>
@@ -1581,8 +1737,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7E42C7D-F581-42F8-AD0E-E228090ADEFE}">
   <dimension ref="A3:W107"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
-      <selection activeCell="R73" sqref="R73"/>
+    <sheetView tabSelected="1" topLeftCell="B57" workbookViewId="0">
+      <selection activeCell="V85" sqref="V85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1592,194 +1748,196 @@
     <col min="5" max="5" width="15.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="14.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="66" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
-      <c r="K4" s="3"/>
-      <c r="L4" s="3"/>
-      <c r="M4" s="3"/>
-      <c r="N4" s="3"/>
-      <c r="O4" s="3"/>
-      <c r="P4" s="3"/>
-      <c r="Q4" s="3"/>
-      <c r="R4" s="3"/>
-      <c r="S4" s="3"/>
-      <c r="T4" s="3"/>
-      <c r="U4" s="3"/>
-      <c r="V4" s="3"/>
-      <c r="W4" s="4"/>
+      <c r="B4" s="67"/>
+      <c r="C4" s="67"/>
+      <c r="D4" s="67"/>
+      <c r="E4" s="67"/>
+      <c r="F4" s="67"/>
+      <c r="G4" s="67"/>
+      <c r="H4" s="67"/>
+      <c r="I4" s="67"/>
+      <c r="J4" s="67"/>
+      <c r="K4" s="67"/>
+      <c r="L4" s="67"/>
+      <c r="M4" s="67"/>
+      <c r="N4" s="67"/>
+      <c r="O4" s="67"/>
+      <c r="P4" s="67"/>
+      <c r="Q4" s="67"/>
+      <c r="R4" s="67"/>
+      <c r="S4" s="67"/>
+      <c r="T4" s="67"/>
+      <c r="U4" s="67"/>
+      <c r="V4" s="67"/>
+      <c r="W4" s="68"/>
     </row>
     <row r="5" spans="1:23" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="5"/>
-      <c r="B5" s="6"/>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
-      <c r="G5" s="6"/>
-      <c r="H5" s="6"/>
-      <c r="I5" s="6"/>
-      <c r="J5" s="6"/>
-      <c r="K5" s="6"/>
-      <c r="L5" s="6"/>
-      <c r="M5" s="6"/>
-      <c r="N5" s="6"/>
-      <c r="O5" s="6"/>
-      <c r="P5" s="6"/>
-      <c r="Q5" s="6"/>
-      <c r="R5" s="6"/>
-      <c r="S5" s="6"/>
-      <c r="T5" s="6"/>
-      <c r="U5" s="6"/>
-      <c r="V5" s="6"/>
-      <c r="W5" s="7"/>
+      <c r="A5" s="69"/>
+      <c r="B5" s="70"/>
+      <c r="C5" s="70"/>
+      <c r="D5" s="70"/>
+      <c r="E5" s="70"/>
+      <c r="F5" s="70"/>
+      <c r="G5" s="70"/>
+      <c r="H5" s="70"/>
+      <c r="I5" s="70"/>
+      <c r="J5" s="70"/>
+      <c r="K5" s="70"/>
+      <c r="L5" s="70"/>
+      <c r="M5" s="70"/>
+      <c r="N5" s="70"/>
+      <c r="O5" s="70"/>
+      <c r="P5" s="70"/>
+      <c r="Q5" s="70"/>
+      <c r="R5" s="70"/>
+      <c r="S5" s="70"/>
+      <c r="T5" s="70"/>
+      <c r="U5" s="70"/>
+      <c r="V5" s="70"/>
+      <c r="W5" s="71"/>
     </row>
     <row r="16" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="17" spans="4:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="L17" s="21" t="s">
+      <c r="L17" s="74" t="s">
         <v>2</v>
       </c>
-      <c r="M17" s="22"/>
-      <c r="N17" s="49">
+      <c r="M17" s="75"/>
+      <c r="N17" s="17">
         <v>3000</v>
       </c>
     </row>
     <row r="18" spans="4:14" x14ac:dyDescent="0.25">
-      <c r="D18" s="30" t="s">
+      <c r="D18" s="90" t="s">
         <v>2</v>
       </c>
-      <c r="E18" s="31"/>
-      <c r="F18" s="32">
+      <c r="E18" s="91"/>
+      <c r="F18" s="8">
         <v>1200</v>
       </c>
-      <c r="L18" s="23" t="s">
+      <c r="L18" s="76" t="s">
         <v>8</v>
       </c>
-      <c r="M18" s="19"/>
-      <c r="N18" s="24">
+      <c r="M18" s="77"/>
+      <c r="N18" s="5">
         <v>0.03</v>
       </c>
     </row>
     <row r="19" spans="4:14" x14ac:dyDescent="0.25">
-      <c r="D19" s="33" t="s">
+      <c r="D19" s="92" t="s">
         <v>4</v>
       </c>
-      <c r="E19" s="34"/>
-      <c r="F19" s="35">
+      <c r="E19" s="93"/>
+      <c r="F19" s="9">
         <v>0.05</v>
       </c>
-      <c r="L19" s="25" t="s">
+      <c r="L19" s="86" t="s">
         <v>10</v>
       </c>
-      <c r="M19" s="17"/>
-      <c r="N19" s="26">
+      <c r="M19" s="87"/>
+      <c r="N19" s="6">
         <v>12</v>
       </c>
     </row>
     <row r="20" spans="4:14" x14ac:dyDescent="0.25">
-      <c r="D20" s="36" t="s">
+      <c r="D20" s="94" t="s">
         <v>3</v>
       </c>
-      <c r="E20" s="37"/>
-      <c r="F20" s="38">
+      <c r="E20" s="95"/>
+      <c r="F20" s="10">
         <v>1</v>
       </c>
-      <c r="L20" s="25" t="s">
+      <c r="L20" s="86" t="s">
         <v>11</v>
       </c>
-      <c r="M20" s="17"/>
-      <c r="N20" s="26">
+      <c r="M20" s="87"/>
+      <c r="N20" s="6">
         <v>1</v>
       </c>
     </row>
     <row r="21" spans="4:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D21" s="39" t="s">
+      <c r="D21" s="96" t="s">
         <v>5</v>
       </c>
-      <c r="E21" s="40"/>
-      <c r="F21" s="41" t="s">
+      <c r="E21" s="97"/>
+      <c r="F21" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="L21" s="25" t="s">
+      <c r="L21" s="86" t="s">
         <v>12</v>
       </c>
-      <c r="M21" s="17"/>
-      <c r="N21" s="50">
+      <c r="M21" s="87"/>
+      <c r="N21" s="18">
         <f>(1+N18/N19)^1 -1</f>
         <v>2.4999999999999467E-3</v>
       </c>
     </row>
     <row r="22" spans="4:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="L22" s="74" t="s">
+      <c r="L22" s="88" t="s">
         <v>9</v>
       </c>
-      <c r="M22" s="75"/>
-      <c r="N22" s="76">
+      <c r="M22" s="89"/>
+      <c r="N22" s="33">
         <f>-PMT(N21,N19,,N17)</f>
         <v>246.5810962754669</v>
       </c>
     </row>
     <row r="23" spans="4:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D23" s="71" t="s">
+      <c r="D23" s="82" t="s">
         <v>7</v>
       </c>
-      <c r="E23" s="72"/>
-      <c r="F23" s="73">
+      <c r="E23" s="83"/>
+      <c r="F23" s="32">
         <f>F18/(1+F19)</f>
         <v>1142.8571428571429</v>
       </c>
     </row>
     <row r="24" spans="4:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D24" s="42" t="s">
+      <c r="D24" s="84" t="s">
         <v>7</v>
       </c>
-      <c r="E24" s="43"/>
-      <c r="F24" s="44">
+      <c r="E24" s="85"/>
+      <c r="F24" s="12">
         <f>-PV(F19,F20,,F18)</f>
         <v>1142.8571428571429</v>
       </c>
     </row>
     <row r="35" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="36" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="21" t="s">
+      <c r="B36" s="74" t="s">
         <v>2</v>
       </c>
-      <c r="C36" s="22"/>
-      <c r="D36" s="49">
+      <c r="C36" s="75"/>
+      <c r="D36" s="17">
         <v>25000</v>
       </c>
-      <c r="K36" s="51" t="s">
+      <c r="K36" s="63" t="s">
         <v>20</v>
       </c>
-      <c r="L36" s="52"/>
-      <c r="M36" s="52"/>
-      <c r="N36" s="77"/>
-      <c r="Q36" s="51" t="s">
+      <c r="L36" s="64"/>
+      <c r="M36" s="64"/>
+      <c r="N36" s="65"/>
+      <c r="Q36" s="63" t="s">
         <v>21</v>
       </c>
-      <c r="R36" s="52"/>
-      <c r="S36" s="52"/>
-      <c r="T36" s="77"/>
+      <c r="R36" s="64"/>
+      <c r="S36" s="64"/>
+      <c r="T36" s="65"/>
     </row>
     <row r="37" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B37" s="23" t="s">
+      <c r="B37" s="76" t="s">
         <v>13</v>
       </c>
-      <c r="C37" s="19"/>
-      <c r="D37" s="24">
+      <c r="C37" s="77"/>
+      <c r="D37" s="5">
         <v>0.04</v>
       </c>
       <c r="U37" t="s">
@@ -1787,55 +1945,55 @@
       </c>
     </row>
     <row r="38" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B38" s="27" t="s">
+      <c r="B38" s="78" t="s">
         <v>3</v>
       </c>
-      <c r="C38" s="28"/>
-      <c r="D38" s="29">
+      <c r="C38" s="79"/>
+      <c r="D38" s="7">
         <v>5</v>
       </c>
       <c r="L38" t="s">
         <v>2</v>
       </c>
-      <c r="M38" s="14">
+      <c r="M38" s="1">
         <v>300</v>
       </c>
-      <c r="R38" s="47" t="s">
+      <c r="R38" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="S38" s="14">
+      <c r="S38" s="1">
         <v>110</v>
       </c>
       <c r="U38">
         <v>1</v>
       </c>
-      <c r="V38" s="46">
+      <c r="V38" s="14">
         <f>PV($S$39,U38,,$S$38)</f>
         <v>-103.77358490566037</v>
       </c>
     </row>
     <row r="39" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="M39" s="46"/>
+      <c r="M39" s="14"/>
       <c r="R39" t="s">
         <v>23</v>
       </c>
-      <c r="S39" s="15">
+      <c r="S39" s="2">
         <v>0.06</v>
       </c>
       <c r="U39">
         <v>2</v>
       </c>
-      <c r="V39" s="46">
+      <c r="V39" s="14">
         <f t="shared" ref="V39:V40" si="0">PV($S$39,U39,,$S$38)</f>
         <v>-97.899608401566383</v>
       </c>
     </row>
     <row r="40" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B40" s="53" t="s">
+      <c r="B40" s="80" t="s">
         <v>14</v>
       </c>
-      <c r="C40" s="54"/>
-      <c r="D40" s="55">
+      <c r="C40" s="81"/>
+      <c r="D40" s="19">
         <f>-PMT(D37,D38,D36)</f>
         <v>5615.6778373258485</v>
       </c>
@@ -1848,843 +2006,1097 @@
       <c r="U40">
         <v>3</v>
       </c>
-      <c r="V40" s="46">
+      <c r="V40" s="14">
         <f t="shared" si="0"/>
         <v>-92.358121133553183</v>
       </c>
     </row>
     <row r="41" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B41" s="58"/>
-      <c r="C41" s="59"/>
-      <c r="D41" s="59"/>
-      <c r="E41" s="59"/>
-      <c r="F41" s="60" t="s">
+      <c r="B41" s="22"/>
+      <c r="C41" s="23"/>
+      <c r="D41" s="23"/>
+      <c r="E41" s="23"/>
+      <c r="F41" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="S41" s="46">
+      <c r="S41" s="14">
         <f>-PV(S39,S40,S38)</f>
         <v>294.03131444078036</v>
       </c>
-      <c r="V41" s="46">
+      <c r="V41" s="14">
         <f>SUM(V38:V40)</f>
         <v>-294.03131444077997</v>
       </c>
     </row>
     <row r="42" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B42" s="61" t="s">
+      <c r="B42" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="C42" s="20" t="s">
+      <c r="C42" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="D42" s="20" t="s">
+      <c r="D42" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="E42" s="56" t="s">
+      <c r="E42" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="F42" s="62">
+      <c r="F42" s="26">
         <f>D36</f>
         <v>25000</v>
       </c>
     </row>
     <row r="43" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B43" s="61">
+      <c r="B43" s="25">
         <v>1</v>
       </c>
-      <c r="C43" s="57">
+      <c r="C43" s="21">
         <f>F42*$D$37</f>
         <v>1000</v>
       </c>
-      <c r="D43" s="48">
+      <c r="D43" s="16">
         <f>$D$40</f>
         <v>5615.6778373258485</v>
       </c>
-      <c r="E43" s="48">
+      <c r="E43" s="16">
         <f>D43-C43</f>
         <v>4615.6778373258485</v>
       </c>
-      <c r="F43" s="63">
+      <c r="F43" s="27">
         <f>F42-E43</f>
         <v>20384.322162674151</v>
       </c>
-      <c r="M43" s="78" t="s">
+      <c r="M43" s="54" t="s">
         <v>24</v>
       </c>
-      <c r="N43" s="78"/>
-      <c r="O43" s="78"/>
-      <c r="P43" s="78"/>
+      <c r="N43" s="54"/>
+      <c r="O43" s="54"/>
+      <c r="P43" s="54"/>
     </row>
     <row r="44" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B44" s="61">
+      <c r="B44" s="25">
         <v>2</v>
       </c>
-      <c r="C44" s="57">
+      <c r="C44" s="21">
         <f t="shared" ref="C44:C47" si="1">F43*$D$37</f>
         <v>815.3728865069661</v>
       </c>
-      <c r="D44" s="48">
+      <c r="D44" s="16">
         <f t="shared" ref="D44:D47" si="2">$D$40</f>
         <v>5615.6778373258485</v>
       </c>
-      <c r="E44" s="48">
+      <c r="E44" s="16">
         <f t="shared" ref="E44:E47" si="3">D44-C44</f>
         <v>4800.3049508188824</v>
       </c>
-      <c r="F44" s="63">
+      <c r="F44" s="27">
         <f t="shared" ref="F44:F47" si="4">F43-E44</f>
         <v>15584.017211855269</v>
       </c>
     </row>
     <row r="45" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B45" s="61">
+      <c r="B45" s="25">
         <v>3</v>
       </c>
-      <c r="C45" s="57">
+      <c r="C45" s="21">
         <f t="shared" si="1"/>
         <v>623.36068847421075</v>
       </c>
-      <c r="D45" s="48">
+      <c r="D45" s="16">
         <f t="shared" si="2"/>
         <v>5615.6778373258485</v>
       </c>
-      <c r="E45" s="48">
+      <c r="E45" s="16">
         <f t="shared" si="3"/>
         <v>4992.3171488516382</v>
       </c>
-      <c r="F45" s="63">
+      <c r="F45" s="27">
         <f t="shared" si="4"/>
         <v>10591.700063003631</v>
       </c>
     </row>
     <row r="46" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B46" s="61">
+      <c r="B46" s="25">
         <v>4</v>
       </c>
-      <c r="C46" s="57">
+      <c r="C46" s="21">
         <f t="shared" si="1"/>
         <v>423.66800252014525</v>
       </c>
-      <c r="D46" s="48">
+      <c r="D46" s="16">
         <f t="shared" si="2"/>
         <v>5615.6778373258485</v>
       </c>
-      <c r="E46" s="48">
+      <c r="E46" s="16">
         <f t="shared" si="3"/>
         <v>5192.0098348057036</v>
       </c>
-      <c r="F46" s="63">
+      <c r="F46" s="27">
         <f t="shared" si="4"/>
         <v>5399.6902281979274</v>
       </c>
     </row>
     <row r="47" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B47" s="64">
+      <c r="B47" s="28">
         <v>5</v>
       </c>
-      <c r="C47" s="65">
+      <c r="C47" s="29">
         <f t="shared" si="1"/>
         <v>215.9876091279171</v>
       </c>
-      <c r="D47" s="66">
+      <c r="D47" s="30">
         <f t="shared" si="2"/>
         <v>5615.6778373258485</v>
       </c>
-      <c r="E47" s="66">
+      <c r="E47" s="30">
         <f t="shared" si="3"/>
         <v>5399.690228197931</v>
       </c>
-      <c r="F47" s="67">
+      <c r="F47" s="7">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="48" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="49" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C49" s="68" t="s">
+      <c r="C49" s="50" t="s">
         <v>19</v>
       </c>
-      <c r="D49" s="69"/>
-      <c r="E49" s="70">
+      <c r="D49" s="51"/>
+      <c r="E49" s="31">
         <f>SUM(C43:C47)</f>
         <v>3078.3891866292392</v>
       </c>
     </row>
     <row r="50" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="51" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A51" s="2" t="s">
+      <c r="A51" s="66" t="s">
         <v>25</v>
       </c>
-      <c r="B51" s="3"/>
-      <c r="C51" s="3"/>
-      <c r="D51" s="3"/>
-      <c r="E51" s="3"/>
-      <c r="F51" s="3"/>
-      <c r="G51" s="3"/>
-      <c r="H51" s="3"/>
-      <c r="I51" s="3"/>
-      <c r="J51" s="3"/>
-      <c r="K51" s="3"/>
-      <c r="L51" s="3"/>
-      <c r="M51" s="3"/>
-      <c r="N51" s="3"/>
-      <c r="O51" s="3"/>
-      <c r="P51" s="3"/>
-      <c r="Q51" s="3"/>
-      <c r="R51" s="3"/>
-      <c r="S51" s="3"/>
-      <c r="T51" s="3"/>
-      <c r="U51" s="3"/>
-      <c r="V51" s="3"/>
-      <c r="W51" s="4"/>
+      <c r="B51" s="67"/>
+      <c r="C51" s="67"/>
+      <c r="D51" s="67"/>
+      <c r="E51" s="67"/>
+      <c r="F51" s="67"/>
+      <c r="G51" s="67"/>
+      <c r="H51" s="67"/>
+      <c r="I51" s="67"/>
+      <c r="J51" s="67"/>
+      <c r="K51" s="67"/>
+      <c r="L51" s="67"/>
+      <c r="M51" s="67"/>
+      <c r="N51" s="67"/>
+      <c r="O51" s="67"/>
+      <c r="P51" s="67"/>
+      <c r="Q51" s="67"/>
+      <c r="R51" s="67"/>
+      <c r="S51" s="67"/>
+      <c r="T51" s="67"/>
+      <c r="U51" s="67"/>
+      <c r="V51" s="67"/>
+      <c r="W51" s="68"/>
     </row>
     <row r="52" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="5"/>
-      <c r="B52" s="6"/>
-      <c r="C52" s="6"/>
-      <c r="D52" s="6"/>
-      <c r="E52" s="6"/>
-      <c r="F52" s="6"/>
-      <c r="G52" s="6"/>
-      <c r="H52" s="6"/>
-      <c r="I52" s="6"/>
-      <c r="J52" s="6"/>
-      <c r="K52" s="6"/>
-      <c r="L52" s="6"/>
-      <c r="M52" s="6"/>
-      <c r="N52" s="6"/>
-      <c r="O52" s="6"/>
-      <c r="P52" s="6"/>
-      <c r="Q52" s="6"/>
-      <c r="R52" s="6"/>
-      <c r="S52" s="6"/>
-      <c r="T52" s="6"/>
-      <c r="U52" s="6"/>
-      <c r="V52" s="6"/>
-      <c r="W52" s="7"/>
-    </row>
-    <row r="71" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="72" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B72" s="80" t="s">
+      <c r="A52" s="69"/>
+      <c r="B52" s="70"/>
+      <c r="C52" s="70"/>
+      <c r="D52" s="70"/>
+      <c r="E52" s="70"/>
+      <c r="F52" s="70"/>
+      <c r="G52" s="70"/>
+      <c r="H52" s="70"/>
+      <c r="I52" s="70"/>
+      <c r="J52" s="70"/>
+      <c r="K52" s="70"/>
+      <c r="L52" s="70"/>
+      <c r="M52" s="70"/>
+      <c r="N52" s="70"/>
+      <c r="O52" s="70"/>
+      <c r="P52" s="70"/>
+      <c r="Q52" s="70"/>
+      <c r="R52" s="70"/>
+      <c r="S52" s="70"/>
+      <c r="T52" s="70"/>
+      <c r="U52" s="70"/>
+      <c r="V52" s="70"/>
+      <c r="W52" s="71"/>
+    </row>
+    <row r="71" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="72" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B72" s="72" t="s">
         <v>26</v>
       </c>
-      <c r="C72" s="81"/>
-      <c r="D72" s="82">
+      <c r="C72" s="73"/>
+      <c r="D72" s="35">
         <v>65000000</v>
       </c>
     </row>
-    <row r="73" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B73" s="83" t="s">
+    <row r="73" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="B73" s="55" t="s">
         <v>8</v>
       </c>
-      <c r="C73" s="79"/>
-      <c r="D73" s="84">
+      <c r="C73" s="56"/>
+      <c r="D73" s="36">
         <v>0.08</v>
       </c>
-      <c r="O73" s="1" t="s">
+      <c r="N73" s="22"/>
+      <c r="O73" s="23"/>
+      <c r="P73" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q73" s="24" t="s">
+        <v>46</v>
+      </c>
+      <c r="S73" s="22"/>
+      <c r="T73" s="23"/>
+      <c r="U73" s="23"/>
+      <c r="V73" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="W73" s="24" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="74" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="B74" s="55" t="s">
+        <v>27</v>
+      </c>
+      <c r="C74" s="56"/>
+      <c r="D74" s="37">
+        <v>2</v>
+      </c>
+      <c r="N74" s="86" t="s">
         <v>47</v>
       </c>
-      <c r="P73" s="1"/>
-      <c r="Q73" t="s">
+      <c r="O74" s="87"/>
+      <c r="P74" s="4">
+        <v>25</v>
+      </c>
+      <c r="Q74" s="6">
+        <v>25</v>
+      </c>
+      <c r="S74" s="86" t="s">
+        <v>61</v>
+      </c>
+      <c r="T74" s="87"/>
+      <c r="U74" s="87"/>
+      <c r="V74" s="108">
+        <v>2E-3</v>
+      </c>
+      <c r="W74" s="109">
+        <v>2E-3</v>
+      </c>
+    </row>
+    <row r="75" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B75" s="57" t="s">
+        <v>3</v>
+      </c>
+      <c r="C75" s="58"/>
+      <c r="D75" s="38">
+        <v>8</v>
+      </c>
+      <c r="N75" s="86" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="74" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B74" s="83" t="s">
-        <v>27</v>
-      </c>
-      <c r="C74" s="79"/>
-      <c r="D74" s="85">
-        <v>2</v>
-      </c>
-      <c r="N74" t="s">
-        <v>45</v>
-      </c>
-      <c r="O74" s="1">
-        <v>25</v>
-      </c>
-      <c r="P74" s="1"/>
-      <c r="Q74">
+      <c r="O75" s="87"/>
+      <c r="P75" s="4">
         <v>65</v>
       </c>
-    </row>
-    <row r="75" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B75" s="86" t="s">
-        <v>3</v>
-      </c>
-      <c r="C75" s="87"/>
-      <c r="D75" s="88">
-        <v>8</v>
-      </c>
-      <c r="N75" t="s">
+      <c r="Q75" s="6">
+        <v>60</v>
+      </c>
+      <c r="S75" s="86" t="s">
+        <v>60</v>
+      </c>
+      <c r="T75" s="87"/>
+      <c r="U75" s="87"/>
+      <c r="V75" s="16">
+        <f>-FV(V74,P78,P82)</f>
+        <v>174677985.10748067</v>
+      </c>
+      <c r="W75" s="110">
+        <f>-FV(W74,Q78,Q82)</f>
+        <v>114144635.19729827</v>
+      </c>
+    </row>
+    <row r="76" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N76" s="86" t="s">
+        <v>49</v>
+      </c>
+      <c r="O76" s="87"/>
+      <c r="P76" s="4">
+        <v>85</v>
+      </c>
+      <c r="Q76" s="6">
+        <v>90</v>
+      </c>
+      <c r="S76" s="78" t="s">
+        <v>62</v>
+      </c>
+      <c r="T76" s="79"/>
+      <c r="U76" s="79"/>
+      <c r="V76" s="30">
+        <f>PMT(V74,P80,-V75)</f>
+        <v>917137.57956119278</v>
+      </c>
+      <c r="W76" s="111">
+        <f>PMT(W74,Q80,-W75)</f>
+        <v>445097.15018392843</v>
+      </c>
+    </row>
+    <row r="77" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A77" s="47" t="s">
+        <v>35</v>
+      </c>
+      <c r="B77" s="60" t="s">
+        <v>28</v>
+      </c>
+      <c r="C77" s="61"/>
+      <c r="D77" s="61"/>
+      <c r="E77" s="61"/>
+      <c r="F77" s="62"/>
+      <c r="H77" s="60" t="s">
+        <v>31</v>
+      </c>
+      <c r="I77" s="61"/>
+      <c r="J77" s="61"/>
+      <c r="K77" s="61"/>
+      <c r="L77" s="62"/>
+      <c r="N77" s="86" t="s">
+        <v>56</v>
+      </c>
+      <c r="O77" s="87"/>
+      <c r="P77" s="4">
+        <f>P75-P74</f>
+        <v>40</v>
+      </c>
+      <c r="Q77" s="6">
+        <f>Q75-Q74</f>
+        <v>35</v>
+      </c>
+      <c r="S77" s="49"/>
+      <c r="T77" s="49"/>
+      <c r="U77" s="49"/>
+      <c r="V77" s="14"/>
+    </row>
+    <row r="78" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="N78" s="86" t="s">
+        <v>57</v>
+      </c>
+      <c r="O78" s="87"/>
+      <c r="P78" s="4">
+        <f>P77*12</f>
+        <v>480</v>
+      </c>
+      <c r="Q78" s="6">
+        <f>Q77*12</f>
+        <v>420</v>
+      </c>
+      <c r="S78" s="22"/>
+      <c r="T78" s="112"/>
+      <c r="U78" s="23"/>
+      <c r="V78" s="23" t="s">
+        <v>64</v>
+      </c>
+      <c r="W78" s="24" t="s">
         <v>46</v>
       </c>
-      <c r="O75" s="1">
-        <v>25</v>
-      </c>
-      <c r="P75" s="1"/>
-      <c r="Q75">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="76" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="77" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A77" s="100" t="s">
-        <v>35</v>
-      </c>
-      <c r="B77" s="92" t="s">
-        <v>28</v>
-      </c>
-      <c r="C77" s="93"/>
-      <c r="D77" s="93"/>
-      <c r="E77" s="93"/>
-      <c r="F77" s="94"/>
-      <c r="H77" s="92" t="s">
-        <v>31</v>
-      </c>
-      <c r="I77" s="93"/>
-      <c r="J77" s="93"/>
-      <c r="K77" s="93"/>
-      <c r="L77" s="94"/>
-    </row>
-    <row r="79" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B79" s="16" t="s">
+    </row>
+    <row r="79" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="B79" s="59" t="s">
         <v>29</v>
       </c>
-      <c r="C79" s="16"/>
-      <c r="D79" s="45">
+      <c r="C79" s="59"/>
+      <c r="D79" s="13">
         <f>EFFECT(D73,D74)</f>
         <v>8.1600000000000117E-2</v>
       </c>
-      <c r="H79" s="1" t="s">
+      <c r="H79" s="49" t="s">
         <v>34</v>
       </c>
-      <c r="I79" s="1"/>
-      <c r="J79" s="14">
+      <c r="I79" s="49"/>
+      <c r="J79" s="1">
         <f>F85</f>
         <v>45245009.51578369</v>
       </c>
-    </row>
-    <row r="80" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B80" s="1" t="s">
+      <c r="N79" s="86" t="s">
+        <v>58</v>
+      </c>
+      <c r="O79" s="87"/>
+      <c r="P79" s="4">
+        <f>P76-P75</f>
+        <v>20</v>
+      </c>
+      <c r="Q79" s="6">
+        <f>Q76-Q75</f>
+        <v>30</v>
+      </c>
+      <c r="S79" s="106" t="s">
+        <v>63</v>
+      </c>
+      <c r="T79" s="113"/>
+      <c r="U79" s="107"/>
+      <c r="V79" s="3">
+        <v>300000</v>
+      </c>
+      <c r="W79" s="39">
+        <v>500000</v>
+      </c>
+    </row>
+    <row r="80" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B80" s="49" t="s">
         <v>14</v>
       </c>
-      <c r="C80" s="1"/>
-      <c r="D80" s="46">
+      <c r="C80" s="49"/>
+      <c r="D80" s="14">
         <f>-PMT(D79,D75,D72)</f>
         <v>11379731.896831045</v>
       </c>
-      <c r="H80" s="1" t="s">
+      <c r="H80" s="49" t="s">
         <v>32</v>
       </c>
-      <c r="I80" s="1"/>
-      <c r="J80" s="15">
+      <c r="I80" s="49"/>
+      <c r="J80" s="2">
         <v>0.05</v>
       </c>
-    </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B81" s="58"/>
-      <c r="C81" s="59"/>
-      <c r="D81" s="59"/>
-      <c r="E81" s="59"/>
-      <c r="F81" s="60" t="s">
+      <c r="N80" s="86" t="s">
+        <v>59</v>
+      </c>
+      <c r="O80" s="87"/>
+      <c r="P80" s="4">
+        <f>12*P79</f>
+        <v>240</v>
+      </c>
+      <c r="Q80" s="6">
+        <f>12*Q79</f>
+        <v>360</v>
+      </c>
+      <c r="S80" s="106" t="s">
+        <v>65</v>
+      </c>
+      <c r="T80" s="113"/>
+      <c r="U80" s="107"/>
+      <c r="V80" s="16">
+        <f>V76+V79</f>
+        <v>1217137.5795611928</v>
+      </c>
+      <c r="W80" s="110">
+        <f>W76+W79</f>
+        <v>945097.15018392843</v>
+      </c>
+    </row>
+    <row r="81" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="B81" s="22"/>
+      <c r="C81" s="23"/>
+      <c r="D81" s="23"/>
+      <c r="E81" s="23"/>
+      <c r="F81" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="H81" s="1" t="s">
+      <c r="H81" s="49" t="s">
         <v>33</v>
       </c>
-      <c r="I81" s="1"/>
+      <c r="I81" s="49"/>
       <c r="J81">
         <v>3</v>
       </c>
-    </row>
-    <row r="82" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B82" s="61" t="s">
+      <c r="N81" s="86" t="s">
+        <v>50</v>
+      </c>
+      <c r="O81" s="87"/>
+      <c r="P81" s="3">
+        <v>1670000</v>
+      </c>
+      <c r="Q81" s="39">
+        <f>P81*0.8</f>
+        <v>1336000</v>
+      </c>
+      <c r="S81" s="106" t="s">
+        <v>66</v>
+      </c>
+      <c r="T81" s="113"/>
+      <c r="U81" s="107"/>
+      <c r="V81" s="16">
+        <f>-PV(V74,P80,V80)</f>
+        <v>231815972.5807614</v>
+      </c>
+      <c r="W81" s="110">
+        <f>-PV(W74,Q80,W80)</f>
+        <v>242369040.98166293</v>
+      </c>
+    </row>
+    <row r="82" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B82" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="C82" s="20" t="s">
+      <c r="C82" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="D82" s="20" t="s">
+      <c r="D82" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="E82" s="56" t="s">
+      <c r="E82" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="F82" s="89">
+      <c r="F82" s="39">
         <f>D72</f>
         <v>65000000</v>
       </c>
-      <c r="H82" s="1" t="s">
+      <c r="H82" s="49" t="s">
         <v>14</v>
       </c>
-      <c r="I82" s="1"/>
-      <c r="J82" s="46">
+      <c r="I82" s="49"/>
+      <c r="J82" s="14">
         <f>-PMT(J80,J81,J79)</f>
         <v>16614355.001017952</v>
       </c>
-    </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B83" s="61">
+      <c r="N82" s="86" t="s">
+        <v>51</v>
+      </c>
+      <c r="O82" s="87"/>
+      <c r="P82" s="3">
+        <f>0.13*P81</f>
+        <v>217100</v>
+      </c>
+      <c r="Q82" s="39">
+        <f>0.13*Q81</f>
+        <v>173680</v>
+      </c>
+      <c r="S82" s="106" t="s">
+        <v>67</v>
+      </c>
+      <c r="T82" s="113"/>
+      <c r="U82" s="107"/>
+      <c r="V82" s="16">
+        <f>-PMT(V74,P78,,V81)</f>
+        <v>288114.42733505159</v>
+      </c>
+      <c r="W82" s="110">
+        <f>-PMT(W74,Q78,,W81)</f>
+        <v>368783.47339701263</v>
+      </c>
+    </row>
+    <row r="83" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B83" s="25">
         <v>1</v>
       </c>
-      <c r="C83" s="48">
+      <c r="C83" s="16">
         <f>F82*$D$79</f>
         <v>5304000.0000000075</v>
       </c>
-      <c r="D83" s="48">
+      <c r="D83" s="16">
         <f>$D$80</f>
         <v>11379731.896831045</v>
       </c>
-      <c r="E83" s="20">
+      <c r="E83" s="4">
         <f>D83-C83</f>
         <v>6075731.8968310375</v>
       </c>
-      <c r="F83" s="89">
+      <c r="F83" s="39">
         <f>F82-E83</f>
         <v>58924268.103168964</v>
       </c>
-      <c r="H83" s="58"/>
-      <c r="I83" s="59"/>
-      <c r="J83" s="59"/>
-      <c r="K83" s="59"/>
-      <c r="L83" s="60" t="s">
+      <c r="H83" s="22"/>
+      <c r="I83" s="23"/>
+      <c r="J83" s="23"/>
+      <c r="K83" s="23"/>
+      <c r="L83" s="24" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B84" s="61">
+      <c r="N83" s="86" t="s">
+        <v>52</v>
+      </c>
+      <c r="O83" s="87"/>
+      <c r="P83" s="3">
+        <f>0.07*P81</f>
+        <v>116900.00000000001</v>
+      </c>
+      <c r="Q83" s="39">
+        <f>0.07*Q81</f>
+        <v>93520.000000000015</v>
+      </c>
+      <c r="S83" s="104" t="s">
+        <v>68</v>
+      </c>
+      <c r="T83" s="114"/>
+      <c r="U83" s="105"/>
+      <c r="V83" s="30">
+        <f>V82-P82</f>
+        <v>71014.427335051587</v>
+      </c>
+      <c r="W83" s="111">
+        <f>W82-Q82</f>
+        <v>195103.47339701263</v>
+      </c>
+    </row>
+    <row r="84" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="B84" s="25">
         <v>2</v>
       </c>
-      <c r="C84" s="48">
+      <c r="C84" s="16">
         <f t="shared" ref="C84:C90" si="5">F83*$D$79</f>
         <v>4808220.2772185942</v>
       </c>
-      <c r="D84" s="48">
+      <c r="D84" s="16">
         <f t="shared" ref="D84:D90" si="6">$D$80</f>
         <v>11379731.896831045</v>
       </c>
-      <c r="E84" s="20">
+      <c r="E84" s="4">
         <f t="shared" ref="E84:E90" si="7">D84-C84</f>
         <v>6571511.6196124507</v>
       </c>
-      <c r="F84" s="89">
+      <c r="F84" s="39">
         <f t="shared" ref="F84:F90" si="8">F83-E84</f>
         <v>52352756.483556516</v>
       </c>
-      <c r="H84" s="61" t="s">
+      <c r="H84" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="I84" s="20" t="s">
+      <c r="I84" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="J84" s="20" t="s">
+      <c r="J84" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="K84" s="20" t="s">
+      <c r="K84" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="L84" s="89">
+      <c r="L84" s="39">
         <f>J79</f>
         <v>45245009.51578369</v>
       </c>
-    </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B85" s="95">
+      <c r="N84" s="86" t="s">
+        <v>53</v>
+      </c>
+      <c r="O84" s="87"/>
+      <c r="P84" s="3">
+        <f>P81-P82-P83</f>
+        <v>1336000</v>
+      </c>
+      <c r="Q84" s="39">
+        <f>Q81-Q82-Q83</f>
+        <v>1068800</v>
+      </c>
+    </row>
+    <row r="85" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="B85" s="42">
         <v>3</v>
       </c>
-      <c r="C85" s="96">
+      <c r="C85" s="43">
         <f t="shared" si="5"/>
         <v>4271984.9290582174</v>
       </c>
-      <c r="D85" s="96">
+      <c r="D85" s="43">
         <f t="shared" si="6"/>
         <v>11379731.896831045</v>
       </c>
-      <c r="E85" s="97">
+      <c r="E85" s="44">
         <f t="shared" si="7"/>
         <v>7107746.9677728275</v>
       </c>
-      <c r="F85" s="98">
+      <c r="F85" s="45">
         <f t="shared" si="8"/>
         <v>45245009.51578369</v>
       </c>
-      <c r="H85" s="61">
+      <c r="H85" s="25">
         <v>1</v>
       </c>
-      <c r="I85" s="18">
+      <c r="I85" s="3">
         <f>L84*$J$80</f>
         <v>2262250.4757891847</v>
       </c>
-      <c r="J85" s="48">
+      <c r="J85" s="16">
         <f>$J$82</f>
         <v>16614355.001017952</v>
       </c>
-      <c r="K85" s="20">
+      <c r="K85" s="4">
         <f>J85-I85</f>
         <v>14352104.525228769</v>
       </c>
-      <c r="L85" s="89">
+      <c r="L85" s="39">
         <f>L84-K85</f>
         <v>30892904.990554921</v>
       </c>
-    </row>
-    <row r="86" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B86" s="61">
+      <c r="N85" s="86" t="s">
+        <v>54</v>
+      </c>
+      <c r="O85" s="87"/>
+      <c r="P85" s="3">
+        <f>0.1*P84</f>
+        <v>133600</v>
+      </c>
+      <c r="Q85" s="39">
+        <f>0.1*Q84</f>
+        <v>106880</v>
+      </c>
+    </row>
+    <row r="86" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B86" s="25">
         <v>4</v>
       </c>
-      <c r="C86" s="48">
+      <c r="C86" s="16">
         <f t="shared" si="5"/>
         <v>3691992.7764879544</v>
       </c>
-      <c r="D86" s="48">
+      <c r="D86" s="16">
         <f t="shared" si="6"/>
         <v>11379731.896831045</v>
       </c>
-      <c r="E86" s="20">
+      <c r="E86" s="4">
         <f t="shared" si="7"/>
         <v>7687739.120343091</v>
       </c>
-      <c r="F86" s="89">
+      <c r="F86" s="39">
         <f t="shared" si="8"/>
         <v>37557270.395440601</v>
       </c>
-      <c r="H86" s="61">
+      <c r="H86" s="25">
         <v>2</v>
       </c>
-      <c r="I86" s="18">
+      <c r="I86" s="3">
         <f t="shared" ref="I86:I87" si="9">L85*$J$80</f>
         <v>1544645.2495277461</v>
       </c>
-      <c r="J86" s="48">
+      <c r="J86" s="16">
         <f t="shared" ref="J86:J87" si="10">$J$82</f>
         <v>16614355.001017952</v>
       </c>
-      <c r="K86" s="20">
+      <c r="K86" s="4">
         <f t="shared" ref="K86:K87" si="11">J86-I86</f>
         <v>15069709.751490206</v>
       </c>
-      <c r="L86" s="89">
+      <c r="L86" s="39">
         <f t="shared" ref="L86:L87" si="12">L85-K86</f>
         <v>15823195.239064716</v>
       </c>
-    </row>
-    <row r="87" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B87" s="61">
+      <c r="N86" s="78" t="s">
+        <v>55</v>
+      </c>
+      <c r="O86" s="79"/>
+      <c r="P86" s="46">
+        <f>P84-P85</f>
+        <v>1202400</v>
+      </c>
+      <c r="Q86" s="41">
+        <f>Q84-Q85</f>
+        <v>961920</v>
+      </c>
+    </row>
+    <row r="87" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B87" s="25">
         <v>5</v>
       </c>
-      <c r="C87" s="48">
+      <c r="C87" s="16">
         <f t="shared" si="5"/>
         <v>3064673.2642679573</v>
       </c>
-      <c r="D87" s="48">
+      <c r="D87" s="16">
         <f t="shared" si="6"/>
         <v>11379731.896831045</v>
       </c>
-      <c r="E87" s="20">
+      <c r="E87" s="4">
         <f t="shared" si="7"/>
         <v>8315058.6325630881</v>
       </c>
-      <c r="F87" s="89">
+      <c r="F87" s="39">
         <f t="shared" si="8"/>
         <v>29242211.762877513</v>
       </c>
-      <c r="H87" s="64">
+      <c r="H87" s="28">
         <v>3</v>
       </c>
-      <c r="I87" s="99">
+      <c r="I87" s="46">
         <f t="shared" si="9"/>
         <v>791159.76195323584</v>
       </c>
-      <c r="J87" s="66">
+      <c r="J87" s="30">
         <f t="shared" si="10"/>
         <v>16614355.001017952</v>
       </c>
-      <c r="K87" s="90">
+      <c r="K87" s="40">
         <f t="shared" si="11"/>
         <v>15823195.239064716</v>
       </c>
-      <c r="L87" s="91">
+      <c r="L87" s="41">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B88" s="61">
+    <row r="88" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="B88" s="25">
         <v>6</v>
       </c>
-      <c r="C88" s="48">
+      <c r="C88" s="16">
         <f t="shared" si="5"/>
         <v>2386164.4798508086</v>
       </c>
-      <c r="D88" s="48">
+      <c r="D88" s="16">
         <f t="shared" si="6"/>
         <v>11379731.896831045</v>
       </c>
-      <c r="E88" s="20">
+      <c r="E88" s="4">
         <f t="shared" si="7"/>
         <v>8993567.4169802368</v>
       </c>
-      <c r="F88" s="89">
+      <c r="F88" s="39">
         <f t="shared" si="8"/>
         <v>20248644.345897276</v>
       </c>
     </row>
-    <row r="89" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B89" s="61">
+    <row r="89" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="B89" s="25">
         <v>7</v>
       </c>
-      <c r="C89" s="48">
+      <c r="C89" s="16">
         <f t="shared" si="5"/>
         <v>1652289.3786252202</v>
       </c>
-      <c r="D89" s="48">
+      <c r="D89" s="16">
         <f t="shared" si="6"/>
         <v>11379731.896831045</v>
       </c>
-      <c r="E89" s="20">
+      <c r="E89" s="4">
         <f t="shared" si="7"/>
         <v>9727442.5182058252</v>
       </c>
-      <c r="F89" s="89">
+      <c r="F89" s="39">
         <f t="shared" si="8"/>
         <v>10521201.827691451</v>
       </c>
     </row>
-    <row r="90" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B90" s="64">
+    <row r="90" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B90" s="28">
         <v>8</v>
       </c>
-      <c r="C90" s="66">
+      <c r="C90" s="30">
         <f t="shared" si="5"/>
         <v>858530.06913962367</v>
       </c>
-      <c r="D90" s="66">
+      <c r="D90" s="30">
         <f t="shared" si="6"/>
         <v>11379731.896831045</v>
       </c>
-      <c r="E90" s="90">
+      <c r="E90" s="40">
         <f t="shared" si="7"/>
         <v>10521201.827691421</v>
       </c>
-      <c r="F90" s="91">
+      <c r="F90" s="41">
         <f t="shared" si="8"/>
         <v>2.9802322387695313E-8</v>
       </c>
     </row>
-    <row r="92" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A92" s="101" t="s">
+    <row r="92" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A92" s="34" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="93" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B93" s="1" t="s">
+    <row r="93" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="B93" s="49" t="s">
         <v>32</v>
       </c>
-      <c r="C93" s="1"/>
-      <c r="D93" s="15">
+      <c r="C93" s="49"/>
+      <c r="D93" s="2">
         <v>0.03</v>
       </c>
     </row>
-    <row r="94" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B94" t="s">
         <v>15</v>
       </c>
-      <c r="C94" s="1" t="s">
+      <c r="C94" s="49" t="s">
         <v>38</v>
       </c>
-      <c r="D94" s="1"/>
-      <c r="E94" s="1" t="s">
+      <c r="D94" s="49"/>
+      <c r="E94" s="49" t="s">
         <v>39</v>
       </c>
-      <c r="F94" s="1"/>
-    </row>
-    <row r="95" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F94" s="49"/>
+    </row>
+    <row r="95" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B95">
         <v>1</v>
       </c>
-      <c r="C95" s="102">
+      <c r="C95" s="52">
         <f>$D$80</f>
         <v>11379731.896831045</v>
       </c>
-      <c r="D95" s="1"/>
-      <c r="E95" s="102">
+      <c r="D95" s="49"/>
+      <c r="E95" s="52">
         <f>-PV($D$93,B95,,C95)</f>
         <v>11048283.394981597</v>
       </c>
-      <c r="F95" s="1"/>
-      <c r="G95" s="46"/>
-    </row>
-    <row r="96" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F95" s="49"/>
+      <c r="G95" s="14"/>
+    </row>
+    <row r="96" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B96">
         <v>2</v>
       </c>
-      <c r="C96" s="102">
+      <c r="C96" s="52">
         <f t="shared" ref="C96:C97" si="13">$D$80</f>
         <v>11379731.896831045</v>
       </c>
-      <c r="D96" s="1"/>
-      <c r="E96" s="102">
+      <c r="D96" s="49"/>
+      <c r="E96" s="52">
         <f t="shared" ref="E96:E100" si="14">-PV($D$93,B96,,C96)</f>
         <v>10726488.732991843</v>
       </c>
-      <c r="F96" s="1"/>
-      <c r="G96" s="46"/>
+      <c r="F96" s="49"/>
+      <c r="G96" s="14"/>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B97">
         <v>3</v>
       </c>
-      <c r="C97" s="102">
+      <c r="C97" s="52">
         <f t="shared" si="13"/>
         <v>11379731.896831045</v>
       </c>
-      <c r="D97" s="1"/>
-      <c r="E97" s="102">
+      <c r="D97" s="49"/>
+      <c r="E97" s="52">
         <f t="shared" si="14"/>
         <v>10414066.731060041</v>
       </c>
-      <c r="F97" s="1"/>
-      <c r="G97" s="46"/>
+      <c r="F97" s="49"/>
+      <c r="G97" s="14"/>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B98">
         <v>4</v>
       </c>
-      <c r="C98" s="102">
+      <c r="C98" s="52">
         <f>$J$82</f>
         <v>16614355.001017952</v>
       </c>
-      <c r="D98" s="1"/>
-      <c r="E98" s="102">
+      <c r="D98" s="49"/>
+      <c r="E98" s="52">
         <f t="shared" si="14"/>
         <v>14761639.227877704</v>
       </c>
-      <c r="F98" s="1"/>
-      <c r="G98" s="46"/>
+      <c r="F98" s="49"/>
+      <c r="G98" s="14"/>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B99">
         <v>5</v>
       </c>
-      <c r="C99" s="102">
+      <c r="C99" s="52">
         <f t="shared" ref="C99:C100" si="15">$J$82</f>
         <v>16614355.001017952</v>
       </c>
-      <c r="D99" s="1"/>
-      <c r="E99" s="102">
+      <c r="D99" s="49"/>
+      <c r="E99" s="52">
         <f t="shared" si="14"/>
         <v>14331688.570755053</v>
       </c>
-      <c r="F99" s="1"/>
-      <c r="G99" s="46"/>
+      <c r="F99" s="49"/>
+      <c r="G99" s="14"/>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B100">
         <v>6</v>
       </c>
-      <c r="C100" s="102">
+      <c r="C100" s="52">
         <f t="shared" si="15"/>
         <v>16614355.001017952</v>
       </c>
-      <c r="D100" s="1"/>
-      <c r="E100" s="102">
+      <c r="D100" s="49"/>
+      <c r="E100" s="52">
         <f t="shared" si="14"/>
         <v>13914260.748305876</v>
       </c>
-      <c r="F100" s="1"/>
-      <c r="G100" s="46"/>
+      <c r="F100" s="49"/>
+      <c r="G100" s="14"/>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B101" s="78" t="s">
+      <c r="B101" s="54" t="s">
         <v>37</v>
       </c>
-      <c r="C101" s="78"/>
-      <c r="D101" s="78"/>
-      <c r="E101" s="103">
+      <c r="C101" s="54"/>
+      <c r="D101" s="54"/>
+      <c r="E101" s="53">
         <f>SUM(E95:F100)</f>
         <v>75196427.405972108</v>
       </c>
-      <c r="F101" s="78"/>
-      <c r="G101" s="46"/>
+      <c r="F101" s="54"/>
+      <c r="G101" s="14"/>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A103" s="101" t="s">
+      <c r="A103" s="34" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C104" s="1" t="s">
+      <c r="C104" s="49" t="s">
         <v>41</v>
       </c>
-      <c r="D104" s="1"/>
-      <c r="E104" s="14">
+      <c r="D104" s="49"/>
+      <c r="E104" s="1">
         <f>F85</f>
         <v>45245009.51578369</v>
       </c>
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C105" s="1" t="s">
+      <c r="C105" s="49" t="s">
         <v>42</v>
       </c>
-      <c r="D105" s="1"/>
+      <c r="D105" s="49"/>
       <c r="E105">
         <v>3</v>
       </c>
     </row>
     <row r="106" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C106" s="1" t="s">
+      <c r="C106" s="49" t="s">
         <v>43</v>
       </c>
-      <c r="D106" s="1"/>
-      <c r="E106" s="15">
+      <c r="D106" s="49"/>
+      <c r="E106" s="2">
         <v>0.01</v>
       </c>
     </row>
     <row r="107" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C107" s="68" t="s">
+      <c r="C107" s="50" t="s">
         <v>44</v>
       </c>
-      <c r="D107" s="69"/>
-      <c r="E107" s="104">
+      <c r="D107" s="51"/>
+      <c r="E107" s="48">
         <f>-FV(E106,E105,,E104)</f>
         <v>46615978.549121447</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="58">
-    <mergeCell ref="C106:D106"/>
-    <mergeCell ref="C107:D107"/>
-    <mergeCell ref="O73:P73"/>
-    <mergeCell ref="O74:P74"/>
-    <mergeCell ref="O75:P75"/>
-    <mergeCell ref="E99:F99"/>
-    <mergeCell ref="E100:F100"/>
-    <mergeCell ref="B93:C93"/>
-    <mergeCell ref="E101:F101"/>
-    <mergeCell ref="C104:D104"/>
-    <mergeCell ref="C105:D105"/>
-    <mergeCell ref="C96:D96"/>
-    <mergeCell ref="C97:D97"/>
-    <mergeCell ref="C98:D98"/>
-    <mergeCell ref="C99:D99"/>
-    <mergeCell ref="C100:D100"/>
-    <mergeCell ref="E94:F94"/>
-    <mergeCell ref="E95:F95"/>
-    <mergeCell ref="E96:F96"/>
-    <mergeCell ref="E97:F97"/>
-    <mergeCell ref="E98:F98"/>
-    <mergeCell ref="H81:I81"/>
-    <mergeCell ref="H82:I82"/>
-    <mergeCell ref="H79:I79"/>
-    <mergeCell ref="B101:D101"/>
-    <mergeCell ref="C94:D94"/>
-    <mergeCell ref="C95:D95"/>
-    <mergeCell ref="B74:C74"/>
-    <mergeCell ref="B75:C75"/>
-    <mergeCell ref="B79:C79"/>
-    <mergeCell ref="B80:C80"/>
-    <mergeCell ref="B77:F77"/>
+  <mergeCells count="77">
+    <mergeCell ref="S80:U80"/>
+    <mergeCell ref="S81:U81"/>
+    <mergeCell ref="S82:U82"/>
+    <mergeCell ref="S83:U83"/>
+    <mergeCell ref="S76:U76"/>
+    <mergeCell ref="S75:U75"/>
+    <mergeCell ref="S74:U74"/>
+    <mergeCell ref="S77:U77"/>
+    <mergeCell ref="S79:U79"/>
+    <mergeCell ref="N85:O85"/>
+    <mergeCell ref="N86:O86"/>
+    <mergeCell ref="N78:O78"/>
+    <mergeCell ref="N77:O77"/>
+    <mergeCell ref="N79:O79"/>
+    <mergeCell ref="N80:O80"/>
+    <mergeCell ref="N82:O82"/>
+    <mergeCell ref="N83:O83"/>
+    <mergeCell ref="N84:O84"/>
+    <mergeCell ref="A4:W5"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="L17:M17"/>
+    <mergeCell ref="L18:M18"/>
+    <mergeCell ref="L21:M21"/>
+    <mergeCell ref="L22:M22"/>
+    <mergeCell ref="L20:M20"/>
+    <mergeCell ref="L19:M19"/>
     <mergeCell ref="H77:L77"/>
     <mergeCell ref="H80:I80"/>
     <mergeCell ref="Q36:T36"/>
@@ -2698,19 +3110,39 @@
     <mergeCell ref="B40:C40"/>
     <mergeCell ref="C49:D49"/>
     <mergeCell ref="K36:N36"/>
-    <mergeCell ref="D23:E23"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="L17:M17"/>
-    <mergeCell ref="L18:M18"/>
-    <mergeCell ref="L21:M21"/>
-    <mergeCell ref="L22:M22"/>
-    <mergeCell ref="L20:M20"/>
-    <mergeCell ref="L19:M19"/>
-    <mergeCell ref="A4:W5"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="N75:O75"/>
+    <mergeCell ref="N76:O76"/>
+    <mergeCell ref="N81:O81"/>
+    <mergeCell ref="B74:C74"/>
+    <mergeCell ref="B75:C75"/>
+    <mergeCell ref="B79:C79"/>
+    <mergeCell ref="B80:C80"/>
+    <mergeCell ref="B77:F77"/>
+    <mergeCell ref="H81:I81"/>
+    <mergeCell ref="H82:I82"/>
+    <mergeCell ref="H79:I79"/>
+    <mergeCell ref="B101:D101"/>
+    <mergeCell ref="C94:D94"/>
+    <mergeCell ref="C95:D95"/>
+    <mergeCell ref="E94:F94"/>
+    <mergeCell ref="E95:F95"/>
+    <mergeCell ref="E96:F96"/>
+    <mergeCell ref="E97:F97"/>
+    <mergeCell ref="E98:F98"/>
+    <mergeCell ref="C106:D106"/>
+    <mergeCell ref="C107:D107"/>
+    <mergeCell ref="N74:O74"/>
+    <mergeCell ref="E99:F99"/>
+    <mergeCell ref="E100:F100"/>
+    <mergeCell ref="B93:C93"/>
+    <mergeCell ref="E101:F101"/>
+    <mergeCell ref="C104:D104"/>
+    <mergeCell ref="C105:D105"/>
+    <mergeCell ref="C96:D96"/>
+    <mergeCell ref="C97:D97"/>
+    <mergeCell ref="C98:D98"/>
+    <mergeCell ref="C99:D99"/>
+    <mergeCell ref="C100:D100"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2728,56 +3160,56 @@
   <sheetData>
     <row r="3" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="98" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="9"/>
-      <c r="C4" s="9"/>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
-      <c r="G4" s="9"/>
-      <c r="H4" s="9"/>
-      <c r="I4" s="9"/>
-      <c r="J4" s="9"/>
-      <c r="K4" s="9"/>
-      <c r="L4" s="9"/>
-      <c r="M4" s="9"/>
-      <c r="N4" s="9"/>
-      <c r="O4" s="9"/>
-      <c r="P4" s="9"/>
-      <c r="Q4" s="9"/>
-      <c r="R4" s="9"/>
-      <c r="S4" s="9"/>
-      <c r="T4" s="9"/>
-      <c r="U4" s="9"/>
-      <c r="V4" s="9"/>
-      <c r="W4" s="10"/>
+      <c r="B4" s="99"/>
+      <c r="C4" s="99"/>
+      <c r="D4" s="99"/>
+      <c r="E4" s="99"/>
+      <c r="F4" s="99"/>
+      <c r="G4" s="99"/>
+      <c r="H4" s="99"/>
+      <c r="I4" s="99"/>
+      <c r="J4" s="99"/>
+      <c r="K4" s="99"/>
+      <c r="L4" s="99"/>
+      <c r="M4" s="99"/>
+      <c r="N4" s="99"/>
+      <c r="O4" s="99"/>
+      <c r="P4" s="99"/>
+      <c r="Q4" s="99"/>
+      <c r="R4" s="99"/>
+      <c r="S4" s="99"/>
+      <c r="T4" s="99"/>
+      <c r="U4" s="99"/>
+      <c r="V4" s="99"/>
+      <c r="W4" s="100"/>
     </row>
     <row r="5" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="11"/>
-      <c r="B5" s="12"/>
-      <c r="C5" s="12"/>
-      <c r="D5" s="12"/>
-      <c r="E5" s="12"/>
-      <c r="F5" s="12"/>
-      <c r="G5" s="12"/>
-      <c r="H5" s="12"/>
-      <c r="I5" s="12"/>
-      <c r="J5" s="12"/>
-      <c r="K5" s="12"/>
-      <c r="L5" s="12"/>
-      <c r="M5" s="12"/>
-      <c r="N5" s="12"/>
-      <c r="O5" s="12"/>
-      <c r="P5" s="12"/>
-      <c r="Q5" s="12"/>
-      <c r="R5" s="12"/>
-      <c r="S5" s="12"/>
-      <c r="T5" s="12"/>
-      <c r="U5" s="12"/>
-      <c r="V5" s="12"/>
-      <c r="W5" s="13"/>
+      <c r="A5" s="101"/>
+      <c r="B5" s="102"/>
+      <c r="C5" s="102"/>
+      <c r="D5" s="102"/>
+      <c r="E5" s="102"/>
+      <c r="F5" s="102"/>
+      <c r="G5" s="102"/>
+      <c r="H5" s="102"/>
+      <c r="I5" s="102"/>
+      <c r="J5" s="102"/>
+      <c r="K5" s="102"/>
+      <c r="L5" s="102"/>
+      <c r="M5" s="102"/>
+      <c r="N5" s="102"/>
+      <c r="O5" s="102"/>
+      <c r="P5" s="102"/>
+      <c r="Q5" s="102"/>
+      <c r="R5" s="102"/>
+      <c r="S5" s="102"/>
+      <c r="T5" s="102"/>
+      <c r="U5" s="102"/>
+      <c r="V5" s="102"/>
+      <c r="W5" s="103"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>